<commit_message>
Prepare DB for connection with OwnCloud
</commit_message>
<xml_diff>
--- a/static/files/students_example.xlsx
+++ b/static/files/students_example.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1611265152" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1611265152" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1611265152" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1611265152"/>
+      <pm:revision xmlns:pm="smNativeData" day="1613163604" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1613163604" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1613163604" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1613163604"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Třída</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Skupina</t>
   </si>
   <si>
+    <t>OwnCloudId</t>
+  </si>
+  <si>
     <t>V3A</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>GRAF1</t>
   </si>
   <si>
+    <t>ID-123456</t>
+  </si>
+  <si>
     <t>V3B</t>
   </si>
   <si>
@@ -77,6 +83,9 @@
   </si>
   <si>
     <t>PROG2</t>
+  </si>
+  <si>
+    <t>ID-789012</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1611265152" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613163604" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -122,7 +131,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1611265152" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613163604" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -137,7 +146,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1611265152" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613163604" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -153,7 +162,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1611265152" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613163604" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -168,7 +177,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1611265152" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613163604" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -177,7 +186,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,7 +205,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1611265152" type="1" fgLvl="100" fgClr="00D8D8D8" bgLvl="0" bgClr="00C0C0C0"/>
+            <pm:shade xmlns:pm="smNativeData" id="1613163604" type="1" fgLvl="100" fgClr="00D8D8D8" bgLvl="0" bgClr="00C0C0C0"/>
           </ext>
         </extLst>
       </patternFill>
@@ -207,24 +216,13 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1611265152" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8D8D8"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1611265152" type="1" fgLvl="100" fgClr="00D8D8D8" bgLvl="0" bgClr="00C0C0C0"/>
+            <pm:shade xmlns:pm="smNativeData" id="1613163604" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -240,7 +238,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152"/>
+          <pm:border xmlns:pm="smNativeData" id="1613163604"/>
         </ext>
       </extLst>
     </border>
@@ -259,7 +257,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152">
+          <pm:border xmlns:pm="smNativeData" id="1613163604">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -283,7 +281,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152">
+          <pm:border xmlns:pm="smNativeData" id="1613163604">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -305,7 +303,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152">
+          <pm:border xmlns:pm="smNativeData" id="1613163604">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -329,26 +327,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1611265152"/>
+          <pm:border xmlns:pm="smNativeData" id="1613163604"/>
         </ext>
       </extLst>
     </border>
@@ -389,10 +368,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1611265152" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1613163604" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1611265152" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1613163604" count="1">
         <pm:color name="Color 24" rgb="D8D8D8"/>
       </pm:colors>
     </ext>
@@ -656,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="7" defaultColWidth="8.535714" defaultRowHeight="15.40"/>
@@ -668,9 +647,10 @@
     <col min="2" max="2" width="12.330357" customWidth="1" style="0"/>
     <col min="3" max="3" width="17.107143" customWidth="1" style="0"/>
     <col min="4" max="4" width="27.776786" customWidth="1" style="0"/>
+    <col min="7" max="7" width="10.910714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -689,52 +669,61 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1611265152" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613163604" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -743,14 +732,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1611265152" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1611265152" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613163604" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613163604" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1611265152" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613163604" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>